<commit_message>
setup for extent report
</commit_message>
<xml_diff>
--- a/ProductNavigation.xlsx
+++ b/ProductNavigation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositories\eclipse-workspace\PLP-Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshal\Desktop\mca-final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875057E0-6B4A-469D-894D-656995865205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97283E7-A6CA-44B2-9397-790AAD2B688B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,24 +22,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>HP LP3065</t>
-  </si>
-  <si>
-    <t>iMac</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>MacBook</t>
-  </si>
-  <si>
-    <t>MacBook Air</t>
   </si>
   <si>
     <t>Canon EOS 5D</t>
   </si>
   <si>
-    <t>Samsung Galaxy Tab 10.1</t>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Apple Cinema 30</t>
   </si>
 </sst>
 </file>
@@ -917,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +929,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -944,18 +938,8 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
+      <c r="A4" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>